<commit_message>
KUDU-38: Summary report (excel): + Fixed: user listed in the excel report need to filter by Viewable User List depends on a role of current user + Fixed: first user and current user need to show on the report too. + Fixed: project with pland=NO need to show on the report to avoid invalid-%CU. +
</commit_message>
<xml_diff>
--- a/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
+++ b/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="8955" tabRatio="341"/>
+    <workbookView windowWidth="20280" windowHeight="3120" tabRatio="341"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,11 +28,11 @@
             <charset val="0"/>
           </rPr>
           <t>JXLS2:
-jx:area(lastCell="B2")</t>
+jx:area(lastCell="D4")</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">JXLS2:
-jx:each(items=”columnHeaderList” var=”header” direction=”RIGHT” lastCell=”B1”)
+jx:each(items=”columnHeaderList” var=”header” direction=”RIGHT” lastCell=”D1”)
 </t>
         </r>
       </text>
@@ -54,13 +54,12 @@
             <rFont val="Times New Roman"/>
             <charset val="0"/>
           </rPr>
-          <t xml:space="preserve">JXLS2: 
-jx:each(items=”itemList” var=”item” lastCell=”B2”)
-</t>
+          <t>JXLS2: 
+jx:each(items=”itemList” var=”item” lastCell=”D2”)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +77,7 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items=”item.amdList” var=”amd” direction=”RIGHT” lastCell=”B2”)</t>
+jx:each(items=”item.amdList” var=”amd” direction=”RIGHT” lastCell=”D2”)</t>
         </r>
       </text>
     </comment>
@@ -87,9 +86,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
   <si>
-    <t>Employee</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Target
+%CU</t>
+  </si>
+  <si>
+    <t>Actual
+%CU</t>
   </si>
   <si>
     <t>${header}</t>
@@ -98,21 +105,34 @@
     <t>${item.name}</t>
   </si>
   <si>
+    <t>${item.targetPercentCU}</t>
+  </si>
+  <si>
+    <t>${item.percentCU}</t>
+  </si>
+  <si>
     <t>${amd}</t>
+  </si>
+  <si>
+    <t>Printed: ${datetime} by ${user}</t>
+  </si>
+  <si>
+    <t>Year : ${year} from ${yearStartDate} to ${yearEndDate}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="#,##0.00;\-#,##0.00"/>
     <numFmt numFmtId="177" formatCode="_-&quot;฿&quot;* #,##0_-;\-&quot;฿&quot;* #,##0_-;_-&quot;฿&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,36 +142,36 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="10"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -176,6 +196,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,61 +225,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,9 +241,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,8 +256,66 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,7 +324,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="3" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF007835"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,19 +384,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,151 +516,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,11 +545,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,17 +575,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,11 +593,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,75 +634,69 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -660,102 +708,115 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,6 +870,11 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="00007835"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1104,35 +1170,72 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="24.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="8.71428571428571" customWidth="1"/>
+    <col min="2" max="4" width="8.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" ht="25.5" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" customHeight="1" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Fixed: file not found alert by Ant! Update Excel Template for Time Sheet Summary Report.
</commit_message>
<xml_diff>
--- a/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
+++ b/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20280" windowHeight="3120" tabRatio="341"/>
+    <workbookView windowWidth="19875" windowHeight="8955" tabRatio="341"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,10 +126,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,##0.00;\-#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;฿&quot;* #,##0_-;\-&quot;฿&quot;* #,##0_-;_-&quot;฿&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;฿&quot;* #,##0_-;\-&quot;฿&quot;* #,##0_-;_-&quot;฿&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="24">
@@ -171,8 +171,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -188,30 +210,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,8 +232,39 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,77 +278,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -336,6 +336,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -348,13 +354,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,13 +468,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,126 +510,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -511,12 +517,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,6 +541,26 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,20 +595,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,26 +627,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,156 +637,156 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -869,6 +869,15 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1173,7 +1182,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1236,6 +1245,12 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:AZ1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>"!A"</formula>
+      <formula>"!ZZZZZ"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
KUDU-57: Time Sheet Summary: Summary Report need to be adjusted (merge column plan and no-plan)
</commit_message>
<xml_diff>
--- a/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
+++ b/front/src/main/webapp/WEB-INF/xlsx/report_mandays.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19875" windowHeight="8955" tabRatio="341"/>
+    <workbookView windowWidth="20370" windowHeight="8955" tabRatio="341"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Time Sheet Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -28,11 +28,11 @@
             <charset val="0"/>
           </rPr>
           <t>JXLS2:
-jx:area(lastCell="D4")</t>
+jx:area(lastCell="E4")</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">JXLS2:
-jx:each(items=”columnHeaderList” var=”header” direction=”RIGHT” lastCell=”D1”)
+jx:each(items=”columnHeaderList” var=”header” direction=”RIGHT” lastCell=”E1”)
 </t>
         </r>
       </text>
@@ -55,11 +55,11 @@
             <charset val="0"/>
           </rPr>
           <t>JXLS2: 
-jx:each(items=”itemList” var=”item” lastCell=”D2”)</t>
+jx:each(items=”itemList” var=”item” lastCell=”E2”)</t>
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items=”item.amdList” var=”amd” direction=”RIGHT” lastCell=”D2”)</t>
+jx:each(items=”item.amdList” var=”amd” direction=”RIGHT” lastCell=”E2”)</t>
         </r>
       </text>
     </comment>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +97,10 @@
   <si>
     <t>Actual
 %CU</t>
+  </si>
+  <si>
+    <t>Final
+%AMD</t>
   </si>
   <si>
     <t>${header}</t>
@@ -111,13 +115,22 @@
     <t>${item.percentCU}</t>
   </si>
   <si>
+    <t>${item.finalPercentAMD}</t>
+  </si>
+  <si>
     <t>${amd}</t>
   </si>
   <si>
-    <t>Printed: ${datetime} by ${user}</t>
+    <t>Printed:</t>
   </si>
   <si>
-    <t>Year : ${year} from ${yearStartDate} to ${yearEndDate}</t>
+    <t xml:space="preserve"> ${datetime}  by ${user}</t>
+  </si>
+  <si>
+    <t>Year :</t>
+  </si>
+  <si>
+    <t>${year}  from  ${yearStartDate}  to  ${yearEndDate}</t>
   </si>
 </sst>
 </file>
@@ -126,13 +139,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="#,##0.00;\-#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;฿&quot;* #,##0_-;\-&quot;฿&quot;* #,##0_-;_-&quot;฿&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;฿&quot;* #,##0.00_-;\-&quot;฿&quot;* #,##0.00_-;_-&quot;฿&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +177,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="8"/>
       <color theme="0" tint="-0.5"/>
       <name val="Calibri"/>
@@ -171,6 +185,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -186,13 +214,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -201,23 +222,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,40 +254,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,6 +283,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -286,36 +330,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,187 +357,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF043868"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,15 +583,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -576,6 +594,48 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,188 +669,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,6 +825,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -811,12 +841,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,7 +899,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -877,11 +907,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
       <color rgb="00007835"/>
+      <color rgb="00043868"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1179,19 +1215,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="24.4285714285714" customWidth="1"/>
-    <col min="2" max="4" width="8.28571428571429" customWidth="1"/>
+    <col min="2" max="5" width="8.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.5" spans="1:4">
+    <row r="1" ht="25.5" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1204,51 +1240,68 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="2" customHeight="1" spans="1:5">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
+      <c r="A3" s="8" t="s">
+        <v>10</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
+      <c r="A4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+    <row r="5" spans="1:4">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D1:AZ1">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>"!A"</formula>
-      <formula>"!ZZZZZ"</formula>
+  <conditionalFormatting sqref="E1:BA1">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>"MA00"</formula>
+      <formula>"MA99"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:BA51 E3:E51">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>